<commit_message>
Code and figure additions to use ASReml BLUPs
</commit_message>
<xml_diff>
--- a/analysis-paper/BLUP_Descriptive_Statistics.xlsx
+++ b/analysis-paper/BLUP_Descriptive_Statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahm543\OneDrive\NSF Common Bean\R\Packages\CDBNgenomics\analysis-paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahm543\Documents\Github\CDBNgenomics\analysis-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="BLUP_Descriptive_Statistics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
   <si>
     <t>Phenotype</t>
   </si>
@@ -146,8 +146,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -629,9 +629,9 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -957,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K14" sqref="K2:K14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +976,7 @@
     <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1007,8 +1007,11 @@
       <c r="L1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>17.0366096232571</v>
       </c>
       <c r="I2" s="2">
-        <f>H2*D2</f>
+        <f t="shared" ref="I2:I22" si="0">H2*D2</f>
         <v>6.854465753962109</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -1043,8 +1046,11 @@
       <c r="K2">
         <v>12045</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>12.724537354416899</v>
       </c>
       <c r="I3" s="2">
-        <f>H3*D3</f>
+        <f t="shared" si="0"/>
         <v>3.0369963694120878</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1079,8 +1085,11 @@
       <c r="K3">
         <v>7544</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>18.148195818419701</v>
       </c>
       <c r="I4" s="2">
-        <f>H4*D4</f>
+        <f t="shared" si="0"/>
         <v>4.439918741027447</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1115,8 +1124,11 @@
       <c r="K4">
         <v>2896</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1142,7 +1154,7 @@
         <v>2990.29198609369</v>
       </c>
       <c r="I5" s="4">
-        <f>H5*D5</f>
+        <f t="shared" si="0"/>
         <v>802.18472822685078</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -1151,8 +1163,11 @@
       <c r="K5">
         <v>2846</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1178,18 +1193,21 @@
         <v>0.34564117887353502</v>
       </c>
       <c r="I6" s="1">
-        <f>H6*D6</f>
+        <f t="shared" si="0"/>
         <v>2.3205452449395758E-2</v>
       </c>
       <c r="J6" s="6">
-        <f>I6/(G6-F6)</f>
+        <f t="shared" ref="J6:J14" si="1">I6/(G6-F6)</f>
         <v>1.1602726224697879E-2</v>
       </c>
       <c r="K6">
         <v>1226</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1215,18 +1233,21 @@
         <v>2.3155878508280101</v>
       </c>
       <c r="I7" s="1">
-        <f>H7*D7</f>
+        <f t="shared" si="0"/>
         <v>0.46391960626138479</v>
       </c>
       <c r="J7" s="6">
-        <f>I7/(G7-F7)</f>
+        <f t="shared" si="1"/>
         <v>6.1855947501517974E-2</v>
       </c>
       <c r="K7">
         <v>1082</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1252,18 +1273,21 @@
         <v>0.95683025091413398</v>
       </c>
       <c r="I8" s="1">
-        <f>H8*D8</f>
+        <f t="shared" si="0"/>
         <v>7.4981371618377715E-2</v>
       </c>
       <c r="J8" s="6">
-        <f>I8/(G8-F8)</f>
+        <f t="shared" si="1"/>
         <v>9.3726714522972144E-3</v>
       </c>
       <c r="K8">
         <v>823</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1289,18 +1313,21 @@
         <v>2.5988981564564702</v>
       </c>
       <c r="I9" s="1">
-        <f>H9*D9</f>
+        <f t="shared" si="0"/>
         <v>0.47972686423123617</v>
       </c>
       <c r="J9" s="6">
-        <f>I9/(G9-F9)</f>
+        <f t="shared" si="1"/>
         <v>0.11993171605780904</v>
       </c>
       <c r="K9">
         <v>664</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1326,18 +1353,21 @@
         <v>1.1169891505587799</v>
       </c>
       <c r="I10" s="1">
-        <f>H10*D10</f>
+        <f t="shared" si="0"/>
         <v>0.22263301006243524</v>
       </c>
       <c r="J10" s="6">
-        <f>I10/(G10-F10)</f>
+        <f t="shared" si="1"/>
         <v>5.5658252515608811E-2</v>
       </c>
       <c r="K10">
         <v>388</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1363,18 +1393,21 @@
         <v>0.84258679070269005</v>
       </c>
       <c r="I11" s="1">
-        <f>H11*D11</f>
+        <f t="shared" si="0"/>
         <v>0.30561105939704447</v>
       </c>
       <c r="J11" s="6">
-        <f>I11/(G11-F11)</f>
+        <f t="shared" si="1"/>
         <v>0.30561105939704447</v>
       </c>
       <c r="K11">
         <v>378</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1400,18 +1433,21 @@
         <v>0.42830971047154698</v>
       </c>
       <c r="I12" s="1">
-        <f>H12*D12</f>
+        <f t="shared" si="0"/>
         <v>6.2105763944583697E-2</v>
       </c>
       <c r="J12" s="6">
-        <f>I12/(G12-F12)</f>
+        <f t="shared" si="1"/>
         <v>6.2105763944583697E-2</v>
       </c>
       <c r="K12">
         <v>378</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1437,18 +1473,21 @@
         <v>2.2514787522457902</v>
       </c>
       <c r="I13" s="1">
-        <f>H13*D13</f>
+        <f t="shared" si="0"/>
         <v>0.2808597898770494</v>
       </c>
       <c r="J13" s="6">
-        <f>I13/(G13-F13)</f>
+        <f t="shared" si="1"/>
         <v>3.5107473734631175E-2</v>
       </c>
       <c r="K13">
         <v>255</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1474,18 +1513,21 @@
         <v>8.9555337729374695</v>
       </c>
       <c r="I14" s="2">
-        <f>H14*D14</f>
+        <f t="shared" si="0"/>
         <v>6.5653301961128907</v>
       </c>
       <c r="J14" s="6">
-        <f>I14/(G14-F14)</f>
+        <f t="shared" si="1"/>
         <v>0.82066627451411134</v>
       </c>
       <c r="K14">
         <v>140</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1511,7 +1553,7 @@
         <v>1727.19142270414</v>
       </c>
       <c r="I15" s="4">
-        <f>H15*D15</f>
+        <f t="shared" si="0"/>
         <v>333.2591089823282</v>
       </c>
       <c r="J15" s="4" t="s">
@@ -1523,8 +1565,11 @@
       <c r="L15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1550,7 +1595,7 @@
         <v>443.182766558644</v>
       </c>
       <c r="I16" s="4">
-        <f>H16*D16</f>
+        <f t="shared" si="0"/>
         <v>303.56963696750233</v>
       </c>
       <c r="J16" s="4" t="s">
@@ -1562,8 +1607,11 @@
       <c r="L16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1589,7 +1637,7 @@
         <v>11.7374236267871</v>
       </c>
       <c r="I17" s="2">
-        <f>H17*D17</f>
+        <f t="shared" si="0"/>
         <v>5.0941140496217905</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -1601,8 +1649,11 @@
       <c r="L17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1628,7 +1679,7 @@
         <v>2.9744038275103502</v>
       </c>
       <c r="I18" s="2">
-        <f>H18*D18</f>
+        <f t="shared" si="0"/>
         <v>1.0223955161066749</v>
       </c>
       <c r="J18" s="6">
@@ -1641,8 +1692,11 @@
       <c r="L18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1668,7 +1722,7 @@
         <v>20.0648032204567</v>
       </c>
       <c r="I19" s="2">
-        <f>H19*D19</f>
+        <f t="shared" si="0"/>
         <v>6.0013102211165199</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -1680,8 +1734,11 @@
       <c r="L19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1707,7 +1764,7 @@
         <v>2.1904360128718099</v>
       </c>
       <c r="I20" s="1">
-        <f>H20*D20</f>
+        <f t="shared" si="0"/>
         <v>1.1154835872291931</v>
       </c>
       <c r="J20" s="6">
@@ -1720,8 +1777,11 @@
       <c r="L20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1747,7 +1807,7 @@
         <v>7.3457426112655302</v>
       </c>
       <c r="I21" s="2">
-        <f>H21*D21</f>
+        <f t="shared" si="0"/>
         <v>4.5587503845703505</v>
       </c>
       <c r="J21" s="6">
@@ -1760,8 +1820,11 @@
       <c r="L21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1787,7 +1850,7 @@
         <v>0.43227604883704501</v>
       </c>
       <c r="I22" s="1">
-        <f>H22*D22</f>
+        <f t="shared" si="0"/>
         <v>6.7951892588056007E-2</v>
       </c>
       <c r="J22" s="6">
@@ -1800,8 +1863,11 @@
       <c r="L22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D25">
         <f>_xlfn.T.TEST(D2:D14,D15:D22,1,2)</f>
         <v>3.6162150889912877E-2</v>

</xml_diff>